<commit_message>
BAARD now saves training data
</commit_message>
<xml_diff>
--- a/tables/breastcancer_svm_1.xlsx
+++ b/tables/breastcancer_svm_1.xlsx
@@ -558,19 +558,19 @@
         <v>0.05</v>
       </c>
       <c r="C4" t="n">
+        <v>91.39784946236557</v>
+      </c>
+      <c r="D4" t="n">
         <v>92.47311827956987</v>
-      </c>
-      <c r="D4" t="n">
-        <v>93.54838709677419</v>
       </c>
       <c r="E4" t="n">
         <v>83.87096774193549</v>
       </c>
       <c r="F4" t="n">
-        <v>9.677419354838712</v>
+        <v>7.526881720430107</v>
       </c>
       <c r="G4" t="n">
-        <v>10.75268817204301</v>
+        <v>7.526881720430107</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
@@ -591,10 +591,10 @@
         <v>4.301075268817205</v>
       </c>
       <c r="F5" t="n">
-        <v>10.75268817204301</v>
+        <v>7.526881720430107</v>
       </c>
       <c r="G5" t="n">
-        <v>10.75268817204301</v>
+        <v>7.526881720430107</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
@@ -615,10 +615,10 @@
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>11.82795698924731</v>
+        <v>7.526881720430107</v>
       </c>
       <c r="G6" t="n">
-        <v>10.75268817204301</v>
+        <v>7.526881720430107</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
@@ -639,10 +639,10 @@
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>11.82795698924731</v>
+        <v>7.526881720430107</v>
       </c>
       <c r="G7" t="n">
-        <v>10.75268817204301</v>
+        <v>7.526881720430107</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
@@ -658,19 +658,19 @@
         <v>0.3</v>
       </c>
       <c r="C8" t="n">
-        <v>70.96774193548387</v>
+        <v>67.74193548387096</v>
       </c>
       <c r="D8" t="n">
-        <v>90.32258064516128</v>
+        <v>91.39784946236557</v>
       </c>
       <c r="E8" t="n">
         <v>34.40860215053764</v>
       </c>
       <c r="F8" t="n">
-        <v>8.60215053763441</v>
+        <v>7.526881720430107</v>
       </c>
       <c r="G8" t="n">
-        <v>11.82795698924731</v>
+        <v>7.526881720430107</v>
       </c>
       <c r="H8" t="n">
         <v>0</v>
@@ -686,19 +686,19 @@
         <v>0.05</v>
       </c>
       <c r="C9" t="n">
-        <v>94.6236559139785</v>
+        <v>91.39784946236557</v>
       </c>
       <c r="D9" t="n">
-        <v>93.54838709677419</v>
+        <v>92.47311827956987</v>
       </c>
       <c r="E9" t="n">
         <v>84.94623655913979</v>
       </c>
       <c r="F9" t="n">
-        <v>11.82795698924731</v>
+        <v>7.526881720430107</v>
       </c>
       <c r="G9" t="n">
-        <v>9.677419354838712</v>
+        <v>7.526881720430107</v>
       </c>
       <c r="H9" t="n">
         <v>0</v>
@@ -719,10 +719,10 @@
         <v>4.301075268817205</v>
       </c>
       <c r="F10" t="n">
-        <v>9.677419354838712</v>
+        <v>7.526881720430107</v>
       </c>
       <c r="G10" t="n">
-        <v>9.677419354838712</v>
+        <v>7.526881720430107</v>
       </c>
       <c r="H10" t="n">
         <v>0</v>
@@ -743,10 +743,10 @@
         <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>9.677419354838712</v>
+        <v>7.526881720430107</v>
       </c>
       <c r="G11" t="n">
-        <v>9.677419354838712</v>
+        <v>7.526881720430107</v>
       </c>
       <c r="H11" t="n">
         <v>0</v>
@@ -767,10 +767,10 @@
         <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>8.60215053763441</v>
+        <v>7.526881720430107</v>
       </c>
       <c r="G12" t="n">
-        <v>8.60215053763441</v>
+        <v>7.526881720430107</v>
       </c>
       <c r="H12" t="n">
         <v>0</v>

</xml_diff>